<commit_message>
upload network and others file
</commit_message>
<xml_diff>
--- a/scrape people/IGuser.xlsx
+++ b/scrape people/IGuser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i7pmonkey/Documents/110_2/專題/scrape people/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6990CA81-5210-9748-9BAE-E4860E6AA5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B6D144-22A5-E749-92CA-E6BF27D4111B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16000" yWindow="500" windowWidth="28260" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -700,9 +700,6 @@
     <t>童仲彥</t>
   </si>
   <si>
-    <t>yu__0429</t>
-  </si>
-  <si>
     <t>金色力量黨</t>
   </si>
   <si>
@@ -722,9 +719,6 @@
   </si>
   <si>
     <t>蔡易餘</t>
-  </si>
-  <si>
-    <t>milly0330</t>
   </si>
   <si>
     <t>邱毅</t>
@@ -1690,6 +1684,12 @@
   <si>
     <t>pay1pay1</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>taiwanatung</t>
+  </si>
+  <si>
+    <t>chiayionefish</t>
   </si>
 </sst>
 </file>
@@ -2084,8 +2084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" zoomScale="175" workbookViewId="0">
-      <selection activeCell="B212" sqref="B212"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="175" workbookViewId="0">
+      <selection activeCell="B172" sqref="B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3753,21 +3753,21 @@
         <v>225</v>
       </c>
       <c r="B169" t="s">
+        <v>554</v>
+      </c>
+      <c r="C169">
+        <v>1</v>
+      </c>
+      <c r="D169" t="s">
         <v>226</v>
-      </c>
-      <c r="C169">
-        <v>1</v>
-      </c>
-      <c r="D169" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="16" customHeight="1">
       <c r="A170" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B170" t="s">
         <v>228</v>
-      </c>
-      <c r="B170" t="s">
-        <v>229</v>
       </c>
       <c r="C170">
         <v>1</v>
@@ -3778,7 +3778,7 @@
     </row>
     <row r="171" spans="1:4" ht="16" customHeight="1">
       <c r="A171" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C171">
         <v>1</v>
@@ -3789,10 +3789,10 @@
     </row>
     <row r="172" spans="1:4" ht="16" customHeight="1">
       <c r="A172" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B172" t="s">
         <v>231</v>
-      </c>
-      <c r="B172" t="s">
-        <v>232</v>
       </c>
       <c r="C172">
         <v>1</v>
@@ -3803,10 +3803,10 @@
     </row>
     <row r="173" spans="1:4" ht="16" customHeight="1">
       <c r="A173" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B173" t="s">
-        <v>234</v>
+        <v>555</v>
       </c>
       <c r="C173">
         <v>1</v>
@@ -3817,7 +3817,7 @@
     </row>
     <row r="174" spans="1:4" ht="16" customHeight="1">
       <c r="A174" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C174">
         <v>1</v>
@@ -3828,7 +3828,7 @@
     </row>
     <row r="175" spans="1:4" ht="16" customHeight="1">
       <c r="A175" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C175">
         <v>1</v>
@@ -3836,7 +3836,7 @@
     </row>
     <row r="176" spans="1:4" ht="16" customHeight="1">
       <c r="A176" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C176">
         <v>1</v>
@@ -3844,10 +3844,10 @@
     </row>
     <row r="177" spans="1:4" ht="16" customHeight="1">
       <c r="A177" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B177" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C177">
         <v>1</v>
@@ -3855,7 +3855,7 @@
     </row>
     <row r="178" spans="1:4" ht="16" customHeight="1">
       <c r="A178" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C178">
         <v>1</v>
@@ -3863,21 +3863,21 @@
     </row>
     <row r="179" spans="1:4" ht="16" customHeight="1">
       <c r="A179" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B179" t="s">
+        <v>240</v>
+      </c>
+      <c r="C179">
+        <v>1</v>
+      </c>
+      <c r="D179" t="s">
         <v>241</v>
-      </c>
-      <c r="B179" t="s">
-        <v>242</v>
-      </c>
-      <c r="C179">
-        <v>1</v>
-      </c>
-      <c r="D179" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="16" customHeight="1">
       <c r="A180" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C180">
         <v>1</v>
@@ -3888,7 +3888,7 @@
     </row>
     <row r="181" spans="1:4" ht="16" customHeight="1">
       <c r="A181" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C181">
         <v>1</v>
@@ -3896,7 +3896,7 @@
     </row>
     <row r="182" spans="1:4" ht="16" customHeight="1">
       <c r="A182" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C182">
         <v>1</v>
@@ -3907,7 +3907,7 @@
     </row>
     <row r="183" spans="1:4" ht="16" customHeight="1">
       <c r="A183" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C183">
         <v>1</v>
@@ -3915,10 +3915,10 @@
     </row>
     <row r="184" spans="1:4" ht="16" customHeight="1">
       <c r="A184" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B184" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C184">
         <v>1</v>
@@ -3929,7 +3929,7 @@
     </row>
     <row r="185" spans="1:4" ht="16" customHeight="1">
       <c r="A185" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C185">
         <v>1</v>
@@ -3937,7 +3937,7 @@
     </row>
     <row r="186" spans="1:4" ht="16" customHeight="1">
       <c r="A186" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C186">
         <v>1</v>
@@ -3945,7 +3945,7 @@
     </row>
     <row r="187" spans="1:4" ht="16" customHeight="1">
       <c r="A187" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C187">
         <v>1</v>
@@ -3953,7 +3953,7 @@
     </row>
     <row r="188" spans="1:4" ht="16" customHeight="1">
       <c r="A188" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C188">
         <v>1</v>
@@ -3964,10 +3964,10 @@
     </row>
     <row r="189" spans="1:4" ht="16" customHeight="1">
       <c r="A189" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B189" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C189">
         <v>1</v>
@@ -3975,10 +3975,10 @@
     </row>
     <row r="190" spans="1:4" ht="16" customHeight="1">
       <c r="A190" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B190" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C190">
         <v>1</v>
@@ -3989,7 +3989,7 @@
     </row>
     <row r="191" spans="1:4" ht="16" customHeight="1">
       <c r="A191" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C191">
         <v>1</v>
@@ -4000,10 +4000,10 @@
     </row>
     <row r="192" spans="1:4" ht="16" customHeight="1">
       <c r="A192" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B192" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C192">
         <v>1</v>
@@ -4011,7 +4011,7 @@
     </row>
     <row r="193" spans="1:4" ht="16" customHeight="1">
       <c r="A193" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C193">
         <v>1</v>
@@ -4019,7 +4019,7 @@
     </row>
     <row r="194" spans="1:4" ht="16" customHeight="1">
       <c r="A194" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C194">
         <v>1</v>
@@ -4030,10 +4030,10 @@
     </row>
     <row r="195" spans="1:4" ht="16" customHeight="1">
       <c r="A195" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B195" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C195">
         <v>1</v>
@@ -4044,7 +4044,7 @@
     </row>
     <row r="196" spans="1:4" ht="16" customHeight="1">
       <c r="A196" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C196">
         <v>1</v>
@@ -4055,18 +4055,18 @@
     </row>
     <row r="197" spans="1:4" ht="16" customHeight="1">
       <c r="A197" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C197">
         <v>1</v>
       </c>
       <c r="D197" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="16" customHeight="1">
       <c r="A198" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C198">
         <v>1</v>
@@ -4074,10 +4074,10 @@
     </row>
     <row r="199" spans="1:4" ht="16" customHeight="1">
       <c r="A199" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B199" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C199">
         <v>1</v>
@@ -4088,7 +4088,7 @@
     </row>
     <row r="200" spans="1:4" ht="16" customHeight="1">
       <c r="A200" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C200">
         <v>1</v>
@@ -4099,7 +4099,7 @@
     </row>
     <row r="201" spans="1:4" ht="16" customHeight="1">
       <c r="A201" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C201">
         <v>1</v>
@@ -4110,7 +4110,7 @@
     </row>
     <row r="202" spans="1:4" ht="16" customHeight="1">
       <c r="A202" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C202">
         <v>1</v>
@@ -4121,7 +4121,7 @@
     </row>
     <row r="203" spans="1:4" ht="16" customHeight="1">
       <c r="A203" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C203">
         <v>1</v>
@@ -4132,7 +4132,7 @@
     </row>
     <row r="204" spans="1:4" ht="16" customHeight="1">
       <c r="A204" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C204">
         <v>1</v>
@@ -4140,7 +4140,7 @@
     </row>
     <row r="205" spans="1:4" ht="16" customHeight="1">
       <c r="A205" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C205">
         <v>1</v>
@@ -4151,7 +4151,7 @@
     </row>
     <row r="206" spans="1:4" ht="16" customHeight="1">
       <c r="A206" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C206">
         <v>1</v>
@@ -4162,7 +4162,7 @@
     </row>
     <row r="207" spans="1:4" ht="16" customHeight="1">
       <c r="A207" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C207">
         <v>1</v>
@@ -4170,10 +4170,10 @@
     </row>
     <row r="208" spans="1:4" ht="16" customHeight="1">
       <c r="A208" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B208" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C208">
         <v>1</v>
@@ -4184,7 +4184,7 @@
     </row>
     <row r="209" spans="1:4" ht="16" customHeight="1">
       <c r="A209" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C209">
         <v>1</v>
@@ -4195,10 +4195,10 @@
     </row>
     <row r="210" spans="1:4" ht="16" customHeight="1">
       <c r="A210" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B210" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C210">
         <v>1</v>
@@ -4209,7 +4209,7 @@
     </row>
     <row r="211" spans="1:4" ht="16" customHeight="1">
       <c r="A211" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C211">
         <v>1</v>
@@ -4220,7 +4220,7 @@
     </row>
     <row r="212" spans="1:4" ht="16" customHeight="1">
       <c r="A212" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C212">
         <v>1</v>
@@ -4228,10 +4228,10 @@
     </row>
     <row r="213" spans="1:4" ht="16" customHeight="1">
       <c r="A213" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B213" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C213">
         <v>1</v>
@@ -4242,7 +4242,7 @@
     </row>
     <row r="214" spans="1:4" ht="16" customHeight="1">
       <c r="A214" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C214">
         <v>1</v>
@@ -4250,7 +4250,7 @@
     </row>
     <row r="215" spans="1:4" ht="16" customHeight="1">
       <c r="A215" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C215">
         <v>1</v>
@@ -4261,7 +4261,7 @@
     </row>
     <row r="216" spans="1:4" ht="16" customHeight="1">
       <c r="A216" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C216">
         <v>1</v>
@@ -4269,7 +4269,7 @@
     </row>
     <row r="217" spans="1:4" ht="16" customHeight="1">
       <c r="A217" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C217">
         <v>1</v>
@@ -4277,7 +4277,7 @@
     </row>
     <row r="218" spans="1:4" ht="16" customHeight="1">
       <c r="A218" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C218">
         <v>1</v>
@@ -4288,10 +4288,10 @@
     </row>
     <row r="219" spans="1:4" ht="16" customHeight="1">
       <c r="A219" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B219" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C219">
         <v>1</v>
@@ -4302,10 +4302,10 @@
     </row>
     <row r="220" spans="1:4" ht="16" customHeight="1">
       <c r="A220" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B220" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C220">
         <v>1</v>
@@ -4316,10 +4316,10 @@
     </row>
     <row r="221" spans="1:4" ht="16" customHeight="1">
       <c r="A221" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B221" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C221">
         <v>1</v>
@@ -4330,7 +4330,7 @@
     </row>
     <row r="222" spans="1:4" ht="16" customHeight="1">
       <c r="A222" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C222">
         <v>1</v>
@@ -4341,7 +4341,7 @@
     </row>
     <row r="223" spans="1:4" ht="16" customHeight="1">
       <c r="A223" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C223">
         <v>1</v>
@@ -4349,7 +4349,7 @@
     </row>
     <row r="224" spans="1:4" ht="16" customHeight="1">
       <c r="A224" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C224">
         <v>1</v>
@@ -4357,7 +4357,7 @@
     </row>
     <row r="225" spans="1:4" ht="16" customHeight="1">
       <c r="A225" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C225">
         <v>1</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="226" spans="1:4" ht="16" customHeight="1">
       <c r="A226" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C226">
         <v>1</v>
@@ -4376,7 +4376,7 @@
     </row>
     <row r="227" spans="1:4" ht="16" customHeight="1">
       <c r="A227" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C227">
         <v>1</v>
@@ -4387,7 +4387,7 @@
     </row>
     <row r="228" spans="1:4" ht="16" customHeight="1">
       <c r="A228" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C228">
         <v>1</v>
@@ -4398,7 +4398,7 @@
     </row>
     <row r="229" spans="1:4" ht="16" customHeight="1">
       <c r="A229" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C229">
         <v>1</v>
@@ -4406,7 +4406,7 @@
     </row>
     <row r="230" spans="1:4" ht="16" customHeight="1">
       <c r="A230" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C230">
         <v>1</v>
@@ -4417,7 +4417,7 @@
     </row>
     <row r="231" spans="1:4" ht="16" customHeight="1">
       <c r="A231" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C231">
         <v>1</v>
@@ -4425,7 +4425,7 @@
     </row>
     <row r="232" spans="1:4" ht="16" customHeight="1">
       <c r="A232" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C232">
         <v>1</v>
@@ -4433,7 +4433,7 @@
     </row>
     <row r="233" spans="1:4" ht="16" customHeight="1">
       <c r="A233" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C233">
         <v>1</v>
@@ -4441,7 +4441,7 @@
     </row>
     <row r="234" spans="1:4" ht="16" customHeight="1">
       <c r="A234" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C234">
         <v>1</v>
@@ -4452,10 +4452,10 @@
     </row>
     <row r="235" spans="1:4" ht="16" customHeight="1">
       <c r="A235" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B235" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C235">
         <v>1</v>
@@ -4463,7 +4463,7 @@
     </row>
     <row r="236" spans="1:4" ht="16" customHeight="1">
       <c r="A236" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C236">
         <v>1</v>
@@ -4471,7 +4471,7 @@
     </row>
     <row r="237" spans="1:4" ht="16" customHeight="1">
       <c r="A237" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C237">
         <v>1</v>
@@ -4479,7 +4479,7 @@
     </row>
     <row r="238" spans="1:4" ht="16" customHeight="1">
       <c r="A238" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C238">
         <v>1</v>
@@ -4490,7 +4490,7 @@
     </row>
     <row r="239" spans="1:4" ht="16" customHeight="1">
       <c r="A239" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C239">
         <v>1</v>
@@ -4501,7 +4501,7 @@
     </row>
     <row r="240" spans="1:4" ht="16" customHeight="1">
       <c r="A240" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C240">
         <v>1</v>
@@ -4509,7 +4509,7 @@
     </row>
     <row r="241" spans="1:4" ht="16" customHeight="1">
       <c r="A241" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C241">
         <v>1</v>
@@ -4520,7 +4520,7 @@
     </row>
     <row r="242" spans="1:4" ht="16" customHeight="1">
       <c r="A242" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C242">
         <v>1</v>
@@ -4528,18 +4528,18 @@
     </row>
     <row r="243" spans="1:4" ht="16" customHeight="1">
       <c r="A243" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C243">
         <v>1</v>
       </c>
       <c r="D243" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="16" customHeight="1">
       <c r="A244" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C244">
         <v>1</v>
@@ -4550,7 +4550,7 @@
     </row>
     <row r="245" spans="1:4" ht="16" customHeight="1">
       <c r="A245" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C245">
         <v>1</v>
@@ -4561,7 +4561,7 @@
     </row>
     <row r="246" spans="1:4" ht="16" customHeight="1">
       <c r="A246" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C246">
         <v>1</v>
@@ -4572,7 +4572,7 @@
     </row>
     <row r="247" spans="1:4" ht="16" customHeight="1">
       <c r="A247" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C247">
         <v>1</v>
@@ -4583,7 +4583,7 @@
     </row>
     <row r="248" spans="1:4" ht="16" customHeight="1">
       <c r="A248" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C248">
         <v>1</v>
@@ -4591,7 +4591,7 @@
     </row>
     <row r="249" spans="1:4" ht="16" customHeight="1">
       <c r="A249" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C249">
         <v>1</v>
@@ -4599,7 +4599,7 @@
     </row>
     <row r="250" spans="1:4" ht="16" customHeight="1">
       <c r="A250" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C250">
         <v>1</v>
@@ -4610,7 +4610,7 @@
     </row>
     <row r="251" spans="1:4" ht="16" customHeight="1">
       <c r="A251" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C251">
         <v>1</v>
@@ -4621,10 +4621,10 @@
     </row>
     <row r="252" spans="1:4" ht="16" customHeight="1">
       <c r="A252" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B252" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C252">
         <v>1</v>
@@ -4635,7 +4635,7 @@
     </row>
     <row r="253" spans="1:4" ht="16" customHeight="1">
       <c r="A253" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C253">
         <v>1</v>
@@ -4643,7 +4643,7 @@
     </row>
     <row r="254" spans="1:4" ht="16" customHeight="1">
       <c r="A254" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C254">
         <v>1</v>
@@ -4651,7 +4651,7 @@
     </row>
     <row r="255" spans="1:4" ht="16" customHeight="1">
       <c r="A255" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C255">
         <v>1</v>
@@ -4659,7 +4659,7 @@
     </row>
     <row r="256" spans="1:4" ht="16" customHeight="1">
       <c r="A256" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C256">
         <v>1</v>
@@ -4670,7 +4670,7 @@
     </row>
     <row r="257" spans="1:4" ht="16" customHeight="1">
       <c r="A257" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C257">
         <v>1</v>
@@ -4678,7 +4678,7 @@
     </row>
     <row r="258" spans="1:4" ht="16" customHeight="1">
       <c r="A258" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C258">
         <v>1</v>
@@ -4689,7 +4689,7 @@
     </row>
     <row r="259" spans="1:4" ht="16" customHeight="1">
       <c r="A259" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C259">
         <v>1</v>
@@ -4697,7 +4697,7 @@
     </row>
     <row r="260" spans="1:4" ht="16" customHeight="1">
       <c r="A260" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C260">
         <v>1</v>
@@ -4708,7 +4708,7 @@
     </row>
     <row r="261" spans="1:4" ht="16" customHeight="1">
       <c r="A261" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C261">
         <v>1</v>
@@ -4716,7 +4716,7 @@
     </row>
     <row r="262" spans="1:4" ht="16" customHeight="1">
       <c r="A262" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C262">
         <v>1</v>
@@ -4724,7 +4724,7 @@
     </row>
     <row r="263" spans="1:4" ht="16" customHeight="1">
       <c r="A263" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C263">
         <v>1</v>
@@ -4732,7 +4732,7 @@
     </row>
     <row r="264" spans="1:4" ht="16" customHeight="1">
       <c r="A264" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C264">
         <v>1</v>
@@ -4740,7 +4740,7 @@
     </row>
     <row r="265" spans="1:4" ht="16" customHeight="1">
       <c r="A265" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C265">
         <v>1</v>
@@ -4751,7 +4751,7 @@
     </row>
     <row r="266" spans="1:4" ht="16" customHeight="1">
       <c r="A266" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C266">
         <v>1</v>
@@ -4759,7 +4759,7 @@
     </row>
     <row r="267" spans="1:4" ht="16" customHeight="1">
       <c r="A267" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C267">
         <v>1</v>
@@ -4767,7 +4767,7 @@
     </row>
     <row r="268" spans="1:4" ht="16" customHeight="1">
       <c r="A268" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C268">
         <v>1</v>
@@ -4775,7 +4775,7 @@
     </row>
     <row r="269" spans="1:4" ht="16" customHeight="1">
       <c r="A269" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C269">
         <v>1</v>
@@ -4786,7 +4786,7 @@
     </row>
     <row r="270" spans="1:4" ht="16" customHeight="1">
       <c r="A270" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C270">
         <v>1</v>
@@ -4794,7 +4794,7 @@
     </row>
     <row r="271" spans="1:4" ht="16" customHeight="1">
       <c r="A271" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C271">
         <v>1</v>
@@ -4802,7 +4802,7 @@
     </row>
     <row r="272" spans="1:4" ht="16" customHeight="1">
       <c r="A272" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C272">
         <v>1</v>
@@ -4810,7 +4810,7 @@
     </row>
     <row r="273" spans="1:4" ht="16" customHeight="1">
       <c r="A273" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C273">
         <v>1</v>
@@ -4818,7 +4818,7 @@
     </row>
     <row r="274" spans="1:4" ht="16" customHeight="1">
       <c r="A274" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C274">
         <v>1</v>
@@ -4829,7 +4829,7 @@
     </row>
     <row r="275" spans="1:4" ht="16" customHeight="1">
       <c r="A275" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C275">
         <v>1</v>
@@ -4837,7 +4837,7 @@
     </row>
     <row r="276" spans="1:4" ht="16" customHeight="1">
       <c r="A276" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C276">
         <v>1</v>
@@ -4845,7 +4845,7 @@
     </row>
     <row r="277" spans="1:4" ht="16" customHeight="1">
       <c r="A277" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C277">
         <v>1</v>
@@ -4853,7 +4853,7 @@
     </row>
     <row r="278" spans="1:4" ht="16" customHeight="1">
       <c r="A278" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C278">
         <v>1</v>
@@ -4861,7 +4861,7 @@
     </row>
     <row r="279" spans="1:4">
       <c r="A279" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C279">
         <v>1</v>
@@ -4869,7 +4869,7 @@
     </row>
     <row r="280" spans="1:4" ht="16" customHeight="1">
       <c r="A280" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C280">
         <v>0</v>
@@ -4877,7 +4877,7 @@
     </row>
     <row r="281" spans="1:4" ht="16" customHeight="1">
       <c r="A281" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C281">
         <v>0</v>
@@ -4885,7 +4885,7 @@
     </row>
     <row r="282" spans="1:4" ht="16" customHeight="1">
       <c r="A282" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C282">
         <v>0</v>
@@ -4893,7 +4893,7 @@
     </row>
     <row r="283" spans="1:4" ht="16" customHeight="1">
       <c r="A283" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C283">
         <v>0</v>
@@ -4901,7 +4901,7 @@
     </row>
     <row r="284" spans="1:4" ht="16" customHeight="1">
       <c r="A284" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C284">
         <v>0</v>
@@ -4909,7 +4909,7 @@
     </row>
     <row r="285" spans="1:4" ht="16" customHeight="1">
       <c r="A285" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C285">
         <v>0</v>
@@ -4917,7 +4917,7 @@
     </row>
     <row r="286" spans="1:4">
       <c r="A286" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C286">
         <v>0</v>
@@ -4925,7 +4925,7 @@
     </row>
     <row r="287" spans="1:4" ht="16" customHeight="1">
       <c r="A287" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C287">
         <v>0</v>
@@ -4933,7 +4933,7 @@
     </row>
     <row r="288" spans="1:4" ht="16" customHeight="1">
       <c r="A288" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C288">
         <v>0</v>
@@ -4941,7 +4941,7 @@
     </row>
     <row r="289" spans="1:3" ht="16" customHeight="1">
       <c r="A289" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C289">
         <v>0</v>
@@ -4949,7 +4949,7 @@
     </row>
     <row r="290" spans="1:3" ht="16" customHeight="1">
       <c r="A290" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C290">
         <v>0</v>
@@ -4957,7 +4957,7 @@
     </row>
     <row r="291" spans="1:3" ht="16" customHeight="1">
       <c r="A291" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C291">
         <v>0</v>
@@ -4965,7 +4965,7 @@
     </row>
     <row r="292" spans="1:3" ht="16" customHeight="1">
       <c r="A292" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C292">
         <v>0</v>
@@ -4973,7 +4973,7 @@
     </row>
     <row r="293" spans="1:3" ht="16" customHeight="1">
       <c r="A293" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C293">
         <v>0</v>
@@ -4981,7 +4981,7 @@
     </row>
     <row r="294" spans="1:3" ht="16" customHeight="1">
       <c r="A294" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C294">
         <v>0</v>
@@ -4989,7 +4989,7 @@
     </row>
     <row r="295" spans="1:3" ht="16" customHeight="1">
       <c r="A295" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C295">
         <v>0</v>
@@ -4997,7 +4997,7 @@
     </row>
     <row r="296" spans="1:3" ht="16" customHeight="1">
       <c r="A296" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C296">
         <v>0</v>
@@ -5005,7 +5005,7 @@
     </row>
     <row r="297" spans="1:3" ht="16" customHeight="1">
       <c r="A297" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C297">
         <v>0</v>
@@ -5013,7 +5013,7 @@
     </row>
     <row r="298" spans="1:3" ht="16" customHeight="1">
       <c r="A298" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C298">
         <v>0</v>
@@ -5021,7 +5021,7 @@
     </row>
     <row r="299" spans="1:3" ht="16" customHeight="1">
       <c r="A299" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C299">
         <v>0</v>
@@ -5029,7 +5029,7 @@
     </row>
     <row r="300" spans="1:3" ht="16" customHeight="1">
       <c r="A300" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C300">
         <v>0</v>
@@ -5037,7 +5037,7 @@
     </row>
     <row r="301" spans="1:3" ht="16" customHeight="1">
       <c r="A301" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C301">
         <v>0</v>
@@ -5045,7 +5045,7 @@
     </row>
     <row r="302" spans="1:3" ht="16" customHeight="1">
       <c r="A302" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C302">
         <v>0</v>
@@ -5053,7 +5053,7 @@
     </row>
     <row r="303" spans="1:3" ht="16" customHeight="1">
       <c r="A303" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C303">
         <v>0</v>
@@ -5061,7 +5061,7 @@
     </row>
     <row r="304" spans="1:3" ht="16" customHeight="1">
       <c r="A304" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C304">
         <v>0</v>
@@ -5069,7 +5069,7 @@
     </row>
     <row r="305" spans="1:3" ht="16" customHeight="1">
       <c r="A305" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C305">
         <v>0</v>
@@ -5077,7 +5077,7 @@
     </row>
     <row r="306" spans="1:3" ht="16" customHeight="1">
       <c r="A306" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C306">
         <v>0</v>
@@ -5085,7 +5085,7 @@
     </row>
     <row r="307" spans="1:3">
       <c r="A307" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C307">
         <v>0</v>
@@ -5093,7 +5093,7 @@
     </row>
     <row r="308" spans="1:3" ht="16" customHeight="1">
       <c r="A308" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C308">
         <v>0</v>
@@ -5101,7 +5101,7 @@
     </row>
     <row r="309" spans="1:3" ht="16" customHeight="1">
       <c r="A309" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C309">
         <v>0</v>
@@ -5109,7 +5109,7 @@
     </row>
     <row r="310" spans="1:3" ht="16" customHeight="1">
       <c r="A310" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C310">
         <v>0</v>
@@ -5117,7 +5117,7 @@
     </row>
     <row r="311" spans="1:3" ht="16" customHeight="1">
       <c r="A311" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C311">
         <v>0</v>
@@ -5125,7 +5125,7 @@
     </row>
     <row r="312" spans="1:3">
       <c r="A312" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C312">
         <v>0</v>
@@ -5133,7 +5133,7 @@
     </row>
     <row r="313" spans="1:3" ht="16" customHeight="1">
       <c r="A313" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C313">
         <v>0</v>
@@ -5141,7 +5141,7 @@
     </row>
     <row r="314" spans="1:3" ht="16" customHeight="1">
       <c r="A314" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C314">
         <v>0</v>
@@ -5149,7 +5149,7 @@
     </row>
     <row r="315" spans="1:3" ht="16" customHeight="1">
       <c r="A315" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C315">
         <v>0</v>
@@ -5157,7 +5157,7 @@
     </row>
     <row r="316" spans="1:3" ht="16" customHeight="1">
       <c r="A316" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C316">
         <v>0</v>
@@ -5165,7 +5165,7 @@
     </row>
     <row r="317" spans="1:3" ht="16" customHeight="1">
       <c r="A317" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C317">
         <v>0</v>
@@ -5173,7 +5173,7 @@
     </row>
     <row r="318" spans="1:3" ht="16" customHeight="1">
       <c r="A318" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C318">
         <v>0</v>
@@ -5181,7 +5181,7 @@
     </row>
     <row r="319" spans="1:3" ht="16" customHeight="1">
       <c r="A319" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C319">
         <v>0</v>
@@ -5189,7 +5189,7 @@
     </row>
     <row r="320" spans="1:3" ht="16" customHeight="1">
       <c r="A320" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C320">
         <v>0</v>
@@ -5197,7 +5197,7 @@
     </row>
     <row r="321" spans="1:3" ht="16" customHeight="1">
       <c r="A321" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C321">
         <v>0</v>
@@ -5205,7 +5205,7 @@
     </row>
     <row r="322" spans="1:3" ht="16" customHeight="1">
       <c r="A322" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C322">
         <v>0</v>
@@ -5213,7 +5213,7 @@
     </row>
     <row r="323" spans="1:3" ht="16" customHeight="1">
       <c r="A323" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C323">
         <v>0</v>
@@ -5221,7 +5221,7 @@
     </row>
     <row r="324" spans="1:3" ht="16" customHeight="1">
       <c r="A324" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C324">
         <v>0</v>
@@ -5229,7 +5229,7 @@
     </row>
     <row r="325" spans="1:3" ht="16" customHeight="1">
       <c r="A325" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C325">
         <v>0</v>
@@ -5237,7 +5237,7 @@
     </row>
     <row r="326" spans="1:3" ht="16" customHeight="1">
       <c r="A326" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C326">
         <v>0</v>
@@ -5245,7 +5245,7 @@
     </row>
     <row r="327" spans="1:3" ht="16" customHeight="1">
       <c r="A327" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C327">
         <v>0</v>
@@ -5253,7 +5253,7 @@
     </row>
     <row r="328" spans="1:3" ht="16" customHeight="1">
       <c r="A328" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C328">
         <v>0</v>
@@ -5261,7 +5261,7 @@
     </row>
     <row r="329" spans="1:3" ht="16" customHeight="1">
       <c r="A329" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C329">
         <v>0</v>
@@ -5269,7 +5269,7 @@
     </row>
     <row r="330" spans="1:3" ht="16" customHeight="1">
       <c r="A330" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C330">
         <v>0</v>
@@ -5277,7 +5277,7 @@
     </row>
     <row r="331" spans="1:3" ht="16" customHeight="1">
       <c r="A331" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C331">
         <v>0</v>
@@ -5285,7 +5285,7 @@
     </row>
     <row r="332" spans="1:3">
       <c r="A332" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C332">
         <v>0</v>
@@ -5293,7 +5293,7 @@
     </row>
     <row r="333" spans="1:3" ht="16" customHeight="1">
       <c r="A333" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C333">
         <v>0</v>
@@ -5301,7 +5301,7 @@
     </row>
     <row r="334" spans="1:3" ht="16" customHeight="1">
       <c r="A334" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C334">
         <v>0</v>
@@ -5309,7 +5309,7 @@
     </row>
     <row r="335" spans="1:3" ht="16" customHeight="1">
       <c r="A335" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C335">
         <v>0</v>
@@ -5317,7 +5317,7 @@
     </row>
     <row r="336" spans="1:3" ht="16" customHeight="1">
       <c r="A336" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C336">
         <v>0</v>
@@ -5325,7 +5325,7 @@
     </row>
     <row r="337" spans="1:3" ht="16" customHeight="1">
       <c r="A337" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C337">
         <v>0</v>
@@ -5333,7 +5333,7 @@
     </row>
     <row r="338" spans="1:3" ht="16" customHeight="1">
       <c r="A338" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C338">
         <v>0</v>
@@ -5341,7 +5341,7 @@
     </row>
     <row r="339" spans="1:3" ht="16" customHeight="1">
       <c r="A339" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C339">
         <v>0</v>
@@ -5349,7 +5349,7 @@
     </row>
     <row r="340" spans="1:3" ht="16" customHeight="1">
       <c r="A340" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C340">
         <v>0</v>
@@ -5357,7 +5357,7 @@
     </row>
     <row r="341" spans="1:3" ht="16" customHeight="1">
       <c r="A341" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C341">
         <v>0</v>
@@ -5365,7 +5365,7 @@
     </row>
     <row r="342" spans="1:3" ht="16" customHeight="1">
       <c r="A342" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C342">
         <v>0</v>
@@ -5373,7 +5373,7 @@
     </row>
     <row r="343" spans="1:3" ht="16" customHeight="1">
       <c r="A343" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C343">
         <v>0</v>
@@ -5381,7 +5381,7 @@
     </row>
     <row r="344" spans="1:3" ht="16" customHeight="1">
       <c r="A344" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C344">
         <v>0</v>
@@ -5389,7 +5389,7 @@
     </row>
     <row r="345" spans="1:3" ht="16" customHeight="1">
       <c r="A345" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C345">
         <v>0</v>
@@ -5397,7 +5397,7 @@
     </row>
     <row r="346" spans="1:3" ht="16" customHeight="1">
       <c r="A346" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C346">
         <v>0</v>
@@ -5405,7 +5405,7 @@
     </row>
     <row r="347" spans="1:3" ht="16" customHeight="1">
       <c r="A347" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C347">
         <v>0</v>
@@ -5413,7 +5413,7 @@
     </row>
     <row r="348" spans="1:3" ht="16" customHeight="1">
       <c r="A348" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C348">
         <v>0</v>
@@ -5421,7 +5421,7 @@
     </row>
     <row r="349" spans="1:3" ht="16" customHeight="1">
       <c r="A349" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C349">
         <v>0</v>
@@ -5429,7 +5429,7 @@
     </row>
     <row r="350" spans="1:3" ht="16" customHeight="1">
       <c r="A350" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C350">
         <v>0</v>
@@ -5437,7 +5437,7 @@
     </row>
     <row r="351" spans="1:3" ht="16" customHeight="1">
       <c r="A351" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C351">
         <v>0</v>
@@ -5445,7 +5445,7 @@
     </row>
     <row r="352" spans="1:3" ht="16" customHeight="1">
       <c r="A352" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C352">
         <v>0</v>
@@ -5453,7 +5453,7 @@
     </row>
     <row r="353" spans="1:3" ht="16" customHeight="1">
       <c r="A353" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C353">
         <v>0</v>
@@ -5461,7 +5461,7 @@
     </row>
     <row r="354" spans="1:3" ht="16" customHeight="1">
       <c r="A354" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C354">
         <v>0</v>
@@ -5469,7 +5469,7 @@
     </row>
     <row r="355" spans="1:3" ht="16" customHeight="1">
       <c r="A355" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C355">
         <v>0</v>
@@ -5477,7 +5477,7 @@
     </row>
     <row r="356" spans="1:3" ht="16" customHeight="1">
       <c r="A356" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C356">
         <v>0</v>
@@ -5485,7 +5485,7 @@
     </row>
     <row r="357" spans="1:3" ht="16" customHeight="1">
       <c r="A357" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C357">
         <v>0</v>
@@ -5493,7 +5493,7 @@
     </row>
     <row r="358" spans="1:3" ht="16" customHeight="1">
       <c r="A358" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C358">
         <v>0</v>
@@ -5501,7 +5501,7 @@
     </row>
     <row r="359" spans="1:3" ht="16" customHeight="1">
       <c r="A359" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C359">
         <v>0</v>
@@ -5509,7 +5509,7 @@
     </row>
     <row r="360" spans="1:3" ht="16" customHeight="1">
       <c r="A360" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C360">
         <v>0</v>
@@ -5517,7 +5517,7 @@
     </row>
     <row r="361" spans="1:3" ht="16" customHeight="1">
       <c r="A361" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C361">
         <v>0</v>
@@ -5525,7 +5525,7 @@
     </row>
     <row r="362" spans="1:3" ht="16" customHeight="1">
       <c r="A362" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C362">
         <v>0</v>
@@ -5533,7 +5533,7 @@
     </row>
     <row r="363" spans="1:3" ht="16" customHeight="1">
       <c r="A363" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C363">
         <v>0</v>
@@ -5541,7 +5541,7 @@
     </row>
     <row r="364" spans="1:3" ht="16" customHeight="1">
       <c r="A364" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C364">
         <v>0</v>
@@ -5549,7 +5549,7 @@
     </row>
     <row r="365" spans="1:3" ht="16" customHeight="1">
       <c r="A365" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C365">
         <v>0</v>
@@ -5557,7 +5557,7 @@
     </row>
     <row r="366" spans="1:3" ht="16" customHeight="1">
       <c r="A366" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C366">
         <v>0</v>
@@ -5565,7 +5565,7 @@
     </row>
     <row r="367" spans="1:3" ht="16" customHeight="1">
       <c r="A367" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C367">
         <v>0</v>
@@ -5573,7 +5573,7 @@
     </row>
     <row r="368" spans="1:3" ht="16" customHeight="1">
       <c r="A368" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C368">
         <v>0</v>
@@ -5581,7 +5581,7 @@
     </row>
     <row r="369" spans="1:3" ht="16" customHeight="1">
       <c r="A369" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C369">
         <v>0</v>
@@ -5589,7 +5589,7 @@
     </row>
     <row r="370" spans="1:3" ht="16" customHeight="1">
       <c r="A370" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C370">
         <v>0</v>
@@ -5597,7 +5597,7 @@
     </row>
     <row r="371" spans="1:3" ht="16" customHeight="1">
       <c r="A371" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C371">
         <v>0</v>
@@ -5605,7 +5605,7 @@
     </row>
     <row r="372" spans="1:3" ht="16" customHeight="1">
       <c r="A372" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C372">
         <v>0</v>
@@ -5613,7 +5613,7 @@
     </row>
     <row r="373" spans="1:3" ht="16" customHeight="1">
       <c r="A373" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C373">
         <v>0</v>
@@ -5621,7 +5621,7 @@
     </row>
     <row r="374" spans="1:3" ht="16" customHeight="1">
       <c r="A374" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C374">
         <v>0</v>
@@ -5629,7 +5629,7 @@
     </row>
     <row r="375" spans="1:3" ht="16" customHeight="1">
       <c r="A375" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C375">
         <v>0</v>
@@ -5637,7 +5637,7 @@
     </row>
     <row r="376" spans="1:3" ht="16" customHeight="1">
       <c r="A376" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C376">
         <v>0</v>
@@ -5645,7 +5645,7 @@
     </row>
     <row r="377" spans="1:3" ht="16" customHeight="1">
       <c r="A377" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C377">
         <v>0</v>
@@ -5653,7 +5653,7 @@
     </row>
     <row r="378" spans="1:3">
       <c r="A378" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C378">
         <v>0</v>
@@ -5661,7 +5661,7 @@
     </row>
     <row r="379" spans="1:3" ht="16" customHeight="1">
       <c r="A379" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C379">
         <v>0</v>
@@ -5669,7 +5669,7 @@
     </row>
     <row r="380" spans="1:3" ht="16" customHeight="1">
       <c r="A380" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C380">
         <v>0</v>
@@ -5677,7 +5677,7 @@
     </row>
     <row r="381" spans="1:3" ht="16" customHeight="1">
       <c r="A381" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C381">
         <v>0</v>
@@ -5685,7 +5685,7 @@
     </row>
     <row r="382" spans="1:3" ht="16" customHeight="1">
       <c r="A382" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C382">
         <v>0</v>
@@ -5693,7 +5693,7 @@
     </row>
     <row r="383" spans="1:3" ht="16" customHeight="1">
       <c r="A383" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C383">
         <v>0</v>
@@ -5701,7 +5701,7 @@
     </row>
     <row r="384" spans="1:3" ht="16" customHeight="1">
       <c r="A384" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C384">
         <v>0</v>
@@ -5709,7 +5709,7 @@
     </row>
     <row r="385" spans="1:3" ht="16" customHeight="1">
       <c r="A385" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C385">
         <v>0</v>
@@ -5717,7 +5717,7 @@
     </row>
     <row r="386" spans="1:3" ht="16" customHeight="1">
       <c r="A386" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C386">
         <v>0</v>
@@ -5725,7 +5725,7 @@
     </row>
     <row r="387" spans="1:3" ht="16" customHeight="1">
       <c r="A387" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C387">
         <v>0</v>
@@ -5733,7 +5733,7 @@
     </row>
     <row r="388" spans="1:3" ht="16" customHeight="1">
       <c r="A388" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C388">
         <v>0</v>
@@ -5741,7 +5741,7 @@
     </row>
     <row r="389" spans="1:3" ht="16" customHeight="1">
       <c r="A389" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C389">
         <v>0</v>
@@ -5749,7 +5749,7 @@
     </row>
     <row r="390" spans="1:3">
       <c r="A390" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C390">
         <v>0</v>
@@ -5757,7 +5757,7 @@
     </row>
     <row r="391" spans="1:3" ht="16" customHeight="1">
       <c r="A391" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C391">
         <v>0</v>
@@ -5765,7 +5765,7 @@
     </row>
     <row r="392" spans="1:3" ht="16" customHeight="1">
       <c r="A392" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C392">
         <v>0</v>
@@ -5773,7 +5773,7 @@
     </row>
     <row r="393" spans="1:3" ht="16" customHeight="1">
       <c r="A393" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C393">
         <v>0</v>
@@ -5781,7 +5781,7 @@
     </row>
     <row r="394" spans="1:3" ht="16" customHeight="1">
       <c r="A394" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C394">
         <v>0</v>
@@ -5789,7 +5789,7 @@
     </row>
     <row r="395" spans="1:3" ht="16" customHeight="1">
       <c r="A395" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C395">
         <v>0</v>
@@ -5797,7 +5797,7 @@
     </row>
     <row r="396" spans="1:3" ht="16" customHeight="1">
       <c r="A396" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C396">
         <v>0</v>
@@ -5805,7 +5805,7 @@
     </row>
     <row r="397" spans="1:3" ht="16" customHeight="1">
       <c r="A397" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C397">
         <v>0</v>
@@ -5813,7 +5813,7 @@
     </row>
     <row r="398" spans="1:3" ht="16" customHeight="1">
       <c r="A398" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C398">
         <v>0</v>
@@ -5821,7 +5821,7 @@
     </row>
     <row r="399" spans="1:3" ht="16" customHeight="1">
       <c r="A399" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C399">
         <v>0</v>
@@ -5829,7 +5829,7 @@
     </row>
     <row r="400" spans="1:3" ht="16" customHeight="1">
       <c r="A400" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C400">
         <v>0</v>
@@ -5837,7 +5837,7 @@
     </row>
     <row r="401" spans="1:3" ht="16" customHeight="1">
       <c r="A401" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C401">
         <v>0</v>
@@ -5845,7 +5845,7 @@
     </row>
     <row r="402" spans="1:3" ht="16" customHeight="1">
       <c r="A402" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C402">
         <v>0</v>
@@ -5853,7 +5853,7 @@
     </row>
     <row r="403" spans="1:3" ht="16" customHeight="1">
       <c r="A403" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C403">
         <v>0</v>
@@ -5861,7 +5861,7 @@
     </row>
     <row r="404" spans="1:3" ht="16" customHeight="1">
       <c r="A404" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C404">
         <v>0</v>
@@ -5869,7 +5869,7 @@
     </row>
     <row r="405" spans="1:3" ht="16" customHeight="1">
       <c r="A405" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C405">
         <v>0</v>
@@ -5877,7 +5877,7 @@
     </row>
     <row r="406" spans="1:3" ht="16" customHeight="1">
       <c r="A406" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C406">
         <v>0</v>
@@ -5885,7 +5885,7 @@
     </row>
     <row r="407" spans="1:3" ht="16" customHeight="1">
       <c r="A407" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C407">
         <v>0</v>
@@ -5893,7 +5893,7 @@
     </row>
     <row r="408" spans="1:3" ht="16" customHeight="1">
       <c r="A408" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C408">
         <v>0</v>
@@ -5901,7 +5901,7 @@
     </row>
     <row r="409" spans="1:3" ht="16" customHeight="1">
       <c r="A409" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C409">
         <v>0</v>
@@ -5909,7 +5909,7 @@
     </row>
     <row r="410" spans="1:3" ht="16" customHeight="1">
       <c r="A410" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C410">
         <v>0</v>
@@ -5917,7 +5917,7 @@
     </row>
     <row r="411" spans="1:3" ht="16" customHeight="1">
       <c r="A411" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C411">
         <v>0</v>
@@ -5925,7 +5925,7 @@
     </row>
     <row r="412" spans="1:3" ht="16" customHeight="1">
       <c r="A412" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C412">
         <v>0</v>
@@ -5933,7 +5933,7 @@
     </row>
     <row r="413" spans="1:3" ht="16" customHeight="1">
       <c r="A413" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C413">
         <v>0</v>
@@ -5941,7 +5941,7 @@
     </row>
     <row r="414" spans="1:3" ht="16" customHeight="1">
       <c r="A414" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C414">
         <v>0</v>
@@ -5949,7 +5949,7 @@
     </row>
     <row r="415" spans="1:3" ht="16" customHeight="1">
       <c r="A415" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C415">
         <v>0</v>
@@ -5957,7 +5957,7 @@
     </row>
     <row r="416" spans="1:3" ht="16" customHeight="1">
       <c r="A416" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C416">
         <v>0</v>
@@ -5965,7 +5965,7 @@
     </row>
     <row r="417" spans="1:3" ht="16" customHeight="1">
       <c r="A417" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C417">
         <v>0</v>
@@ -5973,7 +5973,7 @@
     </row>
     <row r="418" spans="1:3" ht="16" customHeight="1">
       <c r="A418" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C418">
         <v>0</v>
@@ -5981,7 +5981,7 @@
     </row>
     <row r="419" spans="1:3" ht="16" customHeight="1">
       <c r="A419" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C419">
         <v>0</v>
@@ -5989,7 +5989,7 @@
     </row>
     <row r="420" spans="1:3" ht="16" customHeight="1">
       <c r="A420" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C420">
         <v>0</v>
@@ -5997,7 +5997,7 @@
     </row>
     <row r="421" spans="1:3" ht="16" customHeight="1">
       <c r="A421" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C421">
         <v>0</v>
@@ -6005,7 +6005,7 @@
     </row>
     <row r="422" spans="1:3" ht="16" customHeight="1">
       <c r="A422" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C422">
         <v>0</v>
@@ -6013,7 +6013,7 @@
     </row>
     <row r="423" spans="1:3" ht="16" customHeight="1">
       <c r="A423" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C423">
         <v>0</v>
@@ -6021,7 +6021,7 @@
     </row>
     <row r="424" spans="1:3" ht="16" customHeight="1">
       <c r="A424" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C424">
         <v>0</v>
@@ -6029,7 +6029,7 @@
     </row>
     <row r="425" spans="1:3" ht="16" customHeight="1">
       <c r="A425" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C425">
         <v>0</v>
@@ -6037,7 +6037,7 @@
     </row>
     <row r="426" spans="1:3" ht="16" customHeight="1">
       <c r="A426" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C426">
         <v>0</v>
@@ -6045,7 +6045,7 @@
     </row>
     <row r="427" spans="1:3" ht="16" customHeight="1">
       <c r="A427" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C427">
         <v>0</v>
@@ -6053,7 +6053,7 @@
     </row>
     <row r="428" spans="1:3" ht="16" customHeight="1">
       <c r="A428" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C428">
         <v>0</v>
@@ -6061,7 +6061,7 @@
     </row>
     <row r="429" spans="1:3">
       <c r="A429" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C429">
         <v>0</v>
@@ -6069,7 +6069,7 @@
     </row>
     <row r="430" spans="1:3" ht="16" customHeight="1">
       <c r="A430" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C430">
         <v>0</v>
@@ -6077,7 +6077,7 @@
     </row>
     <row r="431" spans="1:3" ht="16" customHeight="1">
       <c r="A431" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C431">
         <v>0</v>
@@ -6085,7 +6085,7 @@
     </row>
     <row r="432" spans="1:3">
       <c r="A432" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C432">
         <v>0</v>
@@ -6093,7 +6093,7 @@
     </row>
     <row r="433" spans="1:3" ht="16" customHeight="1">
       <c r="A433" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C433">
         <v>0</v>
@@ -6101,7 +6101,7 @@
     </row>
     <row r="434" spans="1:3" ht="16" customHeight="1">
       <c r="A434" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C434">
         <v>0</v>
@@ -6109,7 +6109,7 @@
     </row>
     <row r="435" spans="1:3" ht="16" customHeight="1">
       <c r="A435" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C435">
         <v>0</v>
@@ -6117,7 +6117,7 @@
     </row>
     <row r="436" spans="1:3" ht="16" customHeight="1">
       <c r="A436" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C436">
         <v>0</v>
@@ -6125,7 +6125,7 @@
     </row>
     <row r="437" spans="1:3" ht="16" customHeight="1">
       <c r="A437" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C437">
         <v>0</v>
@@ -6133,7 +6133,7 @@
     </row>
     <row r="438" spans="1:3" ht="16" customHeight="1">
       <c r="A438" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C438">
         <v>0</v>
@@ -6141,7 +6141,7 @@
     </row>
     <row r="439" spans="1:3" ht="16" customHeight="1">
       <c r="A439" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C439">
         <v>0</v>
@@ -6149,7 +6149,7 @@
     </row>
     <row r="440" spans="1:3" ht="16" customHeight="1">
       <c r="A440" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C440">
         <v>0</v>
@@ -6157,7 +6157,7 @@
     </row>
     <row r="441" spans="1:3" ht="16" customHeight="1">
       <c r="A441" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C441">
         <v>0</v>
@@ -6165,7 +6165,7 @@
     </row>
     <row r="442" spans="1:3" ht="16" customHeight="1">
       <c r="A442" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C442">
         <v>0</v>
@@ -6173,7 +6173,7 @@
     </row>
     <row r="443" spans="1:3" ht="16" customHeight="1">
       <c r="A443" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C443">
         <v>0</v>
@@ -6181,7 +6181,7 @@
     </row>
     <row r="444" spans="1:3" ht="16" customHeight="1">
       <c r="A444" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C444">
         <v>0</v>
@@ -6189,7 +6189,7 @@
     </row>
     <row r="445" spans="1:3" ht="16" customHeight="1">
       <c r="A445" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C445">
         <v>0</v>
@@ -6197,7 +6197,7 @@
     </row>
     <row r="446" spans="1:3" ht="16" customHeight="1">
       <c r="A446" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C446">
         <v>0</v>
@@ -6205,7 +6205,7 @@
     </row>
     <row r="447" spans="1:3" ht="16" customHeight="1">
       <c r="A447" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C447">
         <v>0</v>
@@ -6213,7 +6213,7 @@
     </row>
     <row r="448" spans="1:3" ht="16" customHeight="1">
       <c r="A448" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C448">
         <v>0</v>
@@ -6221,7 +6221,7 @@
     </row>
     <row r="449" spans="1:3" ht="16" customHeight="1">
       <c r="A449" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C449">
         <v>0</v>
@@ -6229,7 +6229,7 @@
     </row>
     <row r="450" spans="1:3" ht="16" customHeight="1">
       <c r="A450" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C450">
         <v>0</v>
@@ -6237,7 +6237,7 @@
     </row>
     <row r="451" spans="1:3" ht="16" customHeight="1">
       <c r="A451" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C451">
         <v>0</v>
@@ -6245,7 +6245,7 @@
     </row>
     <row r="452" spans="1:3" ht="16" customHeight="1">
       <c r="A452" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C452">
         <v>0</v>
@@ -6253,7 +6253,7 @@
     </row>
     <row r="453" spans="1:3" ht="16" customHeight="1">
       <c r="A453" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C453">
         <v>0</v>
@@ -6261,7 +6261,7 @@
     </row>
     <row r="454" spans="1:3" ht="16" customHeight="1">
       <c r="A454" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C454">
         <v>0</v>
@@ -6269,7 +6269,7 @@
     </row>
     <row r="455" spans="1:3" ht="16" customHeight="1">
       <c r="A455" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C455">
         <v>0</v>
@@ -6277,7 +6277,7 @@
     </row>
     <row r="456" spans="1:3" ht="16" customHeight="1">
       <c r="A456" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C456">
         <v>0</v>
@@ -6285,7 +6285,7 @@
     </row>
     <row r="457" spans="1:3" ht="16" customHeight="1">
       <c r="A457" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C457">
         <v>0</v>
@@ -6293,7 +6293,7 @@
     </row>
     <row r="458" spans="1:3" ht="16" customHeight="1">
       <c r="A458" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C458">
         <v>0</v>
@@ -6301,7 +6301,7 @@
     </row>
     <row r="459" spans="1:3" ht="16" customHeight="1">
       <c r="A459" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C459">
         <v>0</v>
@@ -6309,7 +6309,7 @@
     </row>
     <row r="460" spans="1:3" ht="16" customHeight="1">
       <c r="A460" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C460">
         <v>0</v>
@@ -6317,7 +6317,7 @@
     </row>
     <row r="461" spans="1:3" ht="16" customHeight="1">
       <c r="A461" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C461">
         <v>0</v>
@@ -6325,7 +6325,7 @@
     </row>
     <row r="462" spans="1:3" ht="16" customHeight="1">
       <c r="A462" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C462">
         <v>0</v>
@@ -6333,7 +6333,7 @@
     </row>
     <row r="463" spans="1:3" ht="16" customHeight="1">
       <c r="A463" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C463">
         <v>0</v>
@@ -6341,7 +6341,7 @@
     </row>
     <row r="464" spans="1:3" ht="16" customHeight="1">
       <c r="A464" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C464">
         <v>0</v>
@@ -6349,7 +6349,7 @@
     </row>
     <row r="465" spans="1:3" ht="16" customHeight="1">
       <c r="A465" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C465">
         <v>0</v>
@@ -6357,7 +6357,7 @@
     </row>
     <row r="466" spans="1:3" ht="16" customHeight="1">
       <c r="A466" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C466">
         <v>0</v>
@@ -6365,7 +6365,7 @@
     </row>
     <row r="467" spans="1:3" ht="16" customHeight="1">
       <c r="A467" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C467">
         <v>0</v>
@@ -6373,7 +6373,7 @@
     </row>
     <row r="468" spans="1:3" ht="16" customHeight="1">
       <c r="A468" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C468">
         <v>0</v>
@@ -6381,7 +6381,7 @@
     </row>
     <row r="469" spans="1:3">
       <c r="A469" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C469">
         <v>0</v>
@@ -6389,7 +6389,7 @@
     </row>
     <row r="470" spans="1:3" ht="16" customHeight="1">
       <c r="A470" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C470">
         <v>0</v>
@@ -6397,7 +6397,7 @@
     </row>
     <row r="471" spans="1:3" ht="16" customHeight="1">
       <c r="A471" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C471">
         <v>0</v>
@@ -6405,7 +6405,7 @@
     </row>
     <row r="472" spans="1:3" ht="16" customHeight="1">
       <c r="A472" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C472">
         <v>0</v>
@@ -6413,7 +6413,7 @@
     </row>
     <row r="473" spans="1:3" ht="16" customHeight="1">
       <c r="A473" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C473">
         <v>0</v>
@@ -6421,7 +6421,7 @@
     </row>
     <row r="474" spans="1:3" ht="16" customHeight="1">
       <c r="A474" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C474">
         <v>0</v>
@@ -6429,7 +6429,7 @@
     </row>
     <row r="475" spans="1:3" ht="16" customHeight="1">
       <c r="A475" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C475">
         <v>0</v>
@@ -6437,7 +6437,7 @@
     </row>
     <row r="476" spans="1:3" ht="16" customHeight="1">
       <c r="A476" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C476">
         <v>0</v>

</xml_diff>